<commit_message>
Complete Missing Companies Sorter
</commit_message>
<xml_diff>
--- a/peer_fund_table.xlsx
+++ b/peer_fund_table.xlsx
@@ -1785,7 +1785,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1817,7 +1817,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -1849,7 +1849,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1878,7 +1878,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -1910,7 +1910,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -1939,7 +1939,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -1968,7 +1968,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C8" t="s">
         <v>35</v>
@@ -2000,7 +2000,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -2032,7 +2032,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -2064,7 +2064,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2096,7 +2096,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -2128,7 +2128,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -2160,7 +2160,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -2192,7 +2192,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
@@ -2224,7 +2224,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
@@ -2256,7 +2256,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -2288,7 +2288,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
@@ -2317,7 +2317,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
@@ -2349,7 +2349,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
@@ -2381,7 +2381,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -2413,7 +2413,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
@@ -2445,7 +2445,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
@@ -2474,7 +2474,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -2506,7 +2506,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -2538,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
@@ -2570,7 +2570,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C27" t="s">
         <v>54</v>
@@ -2602,7 +2602,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C28" t="s">
         <v>55</v>
@@ -2634,7 +2634,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
@@ -2666,7 +2666,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C30" t="s">
         <v>57</v>
@@ -2698,7 +2698,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -2730,7 +2730,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C32" t="s">
         <v>59</v>
@@ -2762,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C33" t="s">
         <v>60</v>
@@ -2794,7 +2794,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C34" t="s">
         <v>61</v>
@@ -2826,7 +2826,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C35" t="s">
         <v>62</v>
@@ -2858,7 +2858,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C36" t="s">
         <v>63</v>
@@ -2890,7 +2890,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C37" t="s">
         <v>64</v>
@@ -2922,7 +2922,7 @@
         <v>22</v>
       </c>
       <c r="B38" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C38" t="s">
         <v>65</v>
@@ -2954,7 +2954,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -2986,7 +2986,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C40" t="s">
         <v>67</v>
@@ -3018,7 +3018,7 @@
         <v>17</v>
       </c>
       <c r="B41" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
@@ -3050,7 +3050,7 @@
         <v>27</v>
       </c>
       <c r="B42" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C42" t="s">
         <v>69</v>
@@ -3082,7 +3082,7 @@
         <v>17</v>
       </c>
       <c r="B43" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C43" t="s">
         <v>70</v>
@@ -3114,7 +3114,7 @@
         <v>18</v>
       </c>
       <c r="B44" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
@@ -3146,7 +3146,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C45" t="s">
         <v>72</v>
@@ -3178,7 +3178,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C46" t="s">
         <v>73</v>
@@ -3210,7 +3210,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C47" t="s">
         <v>74</v>
@@ -3239,7 +3239,7 @@
         <v>28</v>
       </c>
       <c r="B48" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C48" t="s">
         <v>75</v>
@@ -3271,7 +3271,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C49" t="s">
         <v>76</v>
@@ -3303,7 +3303,7 @@
         <v>27</v>
       </c>
       <c r="B50" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C50" t="s">
         <v>77</v>
@@ -3335,7 +3335,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C51" t="s">
         <v>78</v>
@@ -3367,7 +3367,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C52" t="s">
         <v>79</v>
@@ -3399,7 +3399,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C53" t="s">
         <v>80</v>
@@ -3428,7 +3428,7 @@
         <v>17</v>
       </c>
       <c r="B54" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C54" t="s">
         <v>81</v>
@@ -3460,7 +3460,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C55" t="s">
         <v>82</v>
@@ -3489,7 +3489,7 @@
         <v>19</v>
       </c>
       <c r="B56" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C56" t="s">
         <v>83</v>
@@ -3521,7 +3521,7 @@
         <v>18</v>
       </c>
       <c r="B57" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C57" t="s">
         <v>84</v>
@@ -3553,7 +3553,7 @@
         <v>19</v>
       </c>
       <c r="B58" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C58" t="s">
         <v>85</v>
@@ -3585,7 +3585,7 @@
         <v>18</v>
       </c>
       <c r="B59" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C59" t="s">
         <v>86</v>
@@ -3617,7 +3617,7 @@
         <v>17</v>
       </c>
       <c r="B60" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C60" t="s">
         <v>87</v>
@@ -3649,7 +3649,7 @@
         <v>22</v>
       </c>
       <c r="B61" s="2">
-        <v>45121</v>
+        <v>45125</v>
       </c>
       <c r="C61" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
Complete Adding New Investment Sheet
</commit_message>
<xml_diff>
--- a/peer_fund_table.xlsx
+++ b/peer_fund_table.xlsx
@@ -1785,7 +1785,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1817,7 +1817,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -1849,7 +1849,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1878,7 +1878,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -1910,7 +1910,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -1939,7 +1939,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -1968,7 +1968,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C8" t="s">
         <v>35</v>
@@ -2000,7 +2000,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -2032,7 +2032,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -2064,7 +2064,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2096,7 +2096,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -2128,7 +2128,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -2160,7 +2160,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -2192,7 +2192,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
@@ -2224,7 +2224,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
@@ -2256,7 +2256,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -2288,7 +2288,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
@@ -2317,7 +2317,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
@@ -2349,7 +2349,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
@@ -2381,7 +2381,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -2413,7 +2413,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
@@ -2445,7 +2445,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
@@ -2474,7 +2474,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -2506,7 +2506,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -2538,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
@@ -2570,7 +2570,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C27" t="s">
         <v>54</v>
@@ -2602,7 +2602,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C28" t="s">
         <v>55</v>
@@ -2634,7 +2634,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C29" t="s">
         <v>56</v>
@@ -2666,7 +2666,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C30" t="s">
         <v>57</v>
@@ -2698,7 +2698,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -2730,7 +2730,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C32" t="s">
         <v>59</v>
@@ -2762,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C33" t="s">
         <v>60</v>
@@ -2794,7 +2794,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C34" t="s">
         <v>61</v>
@@ -2826,7 +2826,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C35" t="s">
         <v>62</v>
@@ -2858,7 +2858,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C36" t="s">
         <v>63</v>
@@ -2890,7 +2890,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C37" t="s">
         <v>64</v>
@@ -2922,7 +2922,7 @@
         <v>22</v>
       </c>
       <c r="B38" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C38" t="s">
         <v>65</v>
@@ -2954,7 +2954,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -2986,7 +2986,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C40" t="s">
         <v>67</v>
@@ -3018,7 +3018,7 @@
         <v>17</v>
       </c>
       <c r="B41" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
@@ -3050,7 +3050,7 @@
         <v>27</v>
       </c>
       <c r="B42" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C42" t="s">
         <v>69</v>
@@ -3082,7 +3082,7 @@
         <v>17</v>
       </c>
       <c r="B43" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C43" t="s">
         <v>70</v>
@@ -3114,7 +3114,7 @@
         <v>18</v>
       </c>
       <c r="B44" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C44" t="s">
         <v>71</v>
@@ -3146,7 +3146,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C45" t="s">
         <v>72</v>
@@ -3178,7 +3178,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C46" t="s">
         <v>73</v>
@@ -3210,7 +3210,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C47" t="s">
         <v>74</v>
@@ -3239,7 +3239,7 @@
         <v>28</v>
       </c>
       <c r="B48" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C48" t="s">
         <v>75</v>
@@ -3271,7 +3271,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C49" t="s">
         <v>76</v>
@@ -3303,7 +3303,7 @@
         <v>27</v>
       </c>
       <c r="B50" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C50" t="s">
         <v>77</v>
@@ -3335,7 +3335,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C51" t="s">
         <v>78</v>
@@ -3367,7 +3367,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C52" t="s">
         <v>79</v>
@@ -3399,7 +3399,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C53" t="s">
         <v>80</v>
@@ -3428,7 +3428,7 @@
         <v>17</v>
       </c>
       <c r="B54" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C54" t="s">
         <v>81</v>
@@ -3460,7 +3460,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C55" t="s">
         <v>82</v>
@@ -3489,7 +3489,7 @@
         <v>19</v>
       </c>
       <c r="B56" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C56" t="s">
         <v>83</v>
@@ -3521,7 +3521,7 @@
         <v>18</v>
       </c>
       <c r="B57" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C57" t="s">
         <v>84</v>
@@ -3553,7 +3553,7 @@
         <v>19</v>
       </c>
       <c r="B58" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C58" t="s">
         <v>85</v>
@@ -3585,7 +3585,7 @@
         <v>18</v>
       </c>
       <c r="B59" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C59" t="s">
         <v>86</v>
@@ -3617,7 +3617,7 @@
         <v>17</v>
       </c>
       <c r="B60" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C60" t="s">
         <v>87</v>
@@ -3649,7 +3649,7 @@
         <v>22</v>
       </c>
       <c r="B61" s="2">
-        <v>45125</v>
+        <v>45126</v>
       </c>
       <c r="C61" t="s">
         <v>88</v>

</xml_diff>